<commit_message>
finished assignment1.py and explanation.pdf
</commit_message>
<xml_diff>
--- a/Assignment1/data-task2.xlsx
+++ b/Assignment1/data-task2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Haider\Documents\Git\FIT2004-S2-2021\Assignment1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\FIT2004-S2-2021\Assignment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{444B1AB6-AC29-4971-81FC-D0FD17133CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE24EB47-9B68-455A-A398-C8760918CDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4200" yWindow="1680" windowWidth="21600" windowHeight="11385" xr2:uid="{3E3F211B-E99D-40EF-9195-86404645BAD2}"/>
+    <workbookView xWindow="-28920" yWindow="7260" windowWidth="29040" windowHeight="15720" xr2:uid="{3E3F211B-E99D-40EF-9195-86404645BAD2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -652,6 +652,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Log(Base)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -717,6 +772,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1162,6 +1272,61 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Base</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1227,6 +1392,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2430,14 +2650,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2465,7 +2685,7 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>700087</xdr:colOff>
+      <xdr:colOff>409575</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
@@ -2833,8 +3053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6733E74-2441-4CAF-A47A-AB6AB96B22BE}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>